<commit_message>
Fix independent deck tuning modes and increase fast tuning speed
- Fix jog wheel channel detection to properly distinguish left/right decks
- Add channel check (1 or 2) in addition to CC check (9 or 10)
- Increase fast tuning speed from 10 kHz to 20 kHz per rotation
- Each deck now correctly uses its own tuning mode (Part A/B)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/config/midi/hercules.xlsx
+++ b/config/midi/hercules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\flex\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\flex\config\midi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7BBFE7-384C-4934-A427-191B622A0AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B04A8E-B74C-41D1-B014-1BCD91630B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" xr2:uid="{34B49229-1ECB-4DC7-BFE8-A0B06FFFBA25}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="98">
   <si>
     <t>cc</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>Change the XIT of Slice 0 or 1 with left or right Tempo Fader (uses same BW configured as rit)</t>
+  </si>
+  <si>
+    <t>toggleTuningMode</t>
+  </si>
+  <si>
+    <t>Cycle through tuning modes: Fine → Coarse → Velocity-based</t>
   </si>
 </sst>
 </file>
@@ -703,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D956A4D3-4253-45EA-9BF7-F7A3D3B9B38F}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1369,7 +1375,7 @@
         <v>6|3</v>
       </c>
       <c r="J15" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="K15" s="8">
         <v>2</v>
@@ -2329,7 +2335,7 @@
         <v>7|3</v>
       </c>
       <c r="J37" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="K37" s="8">
         <v>2</v>
@@ -2880,7 +2886,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F485914A-B60F-4164-B1CA-5A2A7FA4A8F9}">
           <x14:formula1>
-            <xm:f>functions!$A$2:$A$69</xm:f>
+            <xm:f>functions!$A$2:$A$70</xm:f>
           </x14:formula1>
           <xm:sqref>J51 J1:J49</xm:sqref>
         </x14:dataValidation>
@@ -2894,9 +2900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F356390-C5A1-4956-8118-11B48E316739}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3557,7 +3561,7 @@
         <v>6|3</v>
       </c>
       <c r="J15" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="K15" s="8">
         <v>2</v>
@@ -4514,7 +4518,7 @@
         <v>7|3</v>
       </c>
       <c r="J37" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="K37" s="8">
         <v>2</v>
@@ -5065,7 +5069,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A2D9150-9195-4181-AAD2-A5D7BB7BA7B9}">
           <x14:formula1>
-            <xm:f>functions!$A$2:$A$69</xm:f>
+            <xm:f>functions!$A$2:$A$70</xm:f>
           </x14:formula1>
           <xm:sqref>J51 J1:J49</xm:sqref>
         </x14:dataValidation>
@@ -5077,15 +5081,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731D5E7-1A5C-4C46-A916-A5AC3FB36FB7}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
     <col min="4" max="4" width="116" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5259,81 +5263,91 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>